<commit_message>
Even gecheckt of de qmatrix ook echt wordt aangepast door de tijd van aanpassing te controleren. Het werkt
</commit_message>
<xml_diff>
--- a/data/bp2.xlsx
+++ b/data/bp2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>hints</t>
   </si>
@@ -31,22 +31,13 @@
     <t>True</t>
   </si>
   <si>
-    <t>Lie</t>
-  </si>
-  <si>
     <t>Scissors</t>
   </si>
   <si>
-    <t>Paper</t>
-  </si>
-  <si>
     <t>Rock</t>
   </si>
   <si>
-    <t>Player wins</t>
-  </si>
-  <si>
-    <t>Tie</t>
+    <t>Robot won</t>
   </si>
 </sst>
 </file>
@@ -404,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,47 +423,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>